<commit_message>
Updated and adding merged files
</commit_message>
<xml_diff>
--- a/manual test cases/Cartpage_test_cases.xlsx
+++ b/manual test cases/Cartpage_test_cases.xlsx
@@ -5,16 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Shopizer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Shopizer\manual test cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9968110-67F4-4828-B7F2-8D1083F072A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FD96EEA-5EC8-4C4C-B848-1630EF5C8483}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenario" sheetId="1" r:id="rId1"/>
-    <sheet name="Test Case" sheetId="2" r:id="rId2"/>
+    <sheet name="CartTCs" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -446,14 +446,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -737,8 +737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -950,7 +950,7 @@
   <dimension ref="A1:K54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+      <selection activeCell="C12" sqref="C12:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1045,7 +1045,7 @@
       <c r="E3" s="2">
         <v>2</v>
       </c>
-      <c r="F3" s="26" t="s">
+      <c r="F3" s="27" t="s">
         <v>19</v>
       </c>
       <c r="H3" s="23"/>
@@ -1055,7 +1055,7 @@
       <c r="D4" t="s">
         <v>37</v>
       </c>
-      <c r="F4" s="26"/>
+      <c r="F4" s="27"/>
     </row>
     <row r="5" spans="1:11" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="D5" s="16" t="s">
@@ -1127,7 +1127,7 @@
       <c r="D9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F9" s="26"/>
+      <c r="F9" s="27"/>
       <c r="H9" s="25"/>
     </row>
     <row r="10" spans="1:11" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
@@ -1157,7 +1157,7 @@
       <c r="C12" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="D12" s="26" t="s">
+      <c r="D12" s="27" t="s">
         <v>39</v>
       </c>
       <c r="E12" s="2">
@@ -1249,7 +1249,7 @@
       <c r="G17" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="H17" s="28" t="s">
+      <c r="H17" s="26" t="s">
         <v>35</v>
       </c>
       <c r="I17" s="11" t="s">
@@ -1271,7 +1271,7 @@
       <c r="F18" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="H18" s="28"/>
+      <c r="H18" s="26"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="D19" s="1" t="s">
@@ -1283,7 +1283,7 @@
       <c r="F19" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H19" s="28"/>
+      <c r="H19" s="26"/>
     </row>
     <row r="20" spans="1:11" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="D20" s="20" t="s">
@@ -1341,7 +1341,7 @@
       <c r="E24" s="2">
         <v>2</v>
       </c>
-      <c r="F24" s="26" t="s">
+      <c r="F24" s="27" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1349,7 +1349,7 @@
       <c r="D25" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="F25" s="27"/>
+      <c r="F25" s="28"/>
     </row>
     <row r="26" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D26" s="16"/>
@@ -1492,6 +1492,20 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="I32:I34"/>
+    <mergeCell ref="K32:K34"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="H7:H9"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="F33:F34"/>
+    <mergeCell ref="H32:H34"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="F24:F25"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="H22:H23"/>
@@ -1507,20 +1521,6 @@
     <mergeCell ref="F22:F23"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D13"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="F33:F34"/>
-    <mergeCell ref="H32:H34"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="I32:I34"/>
-    <mergeCell ref="K32:K34"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="H7:H9"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="D2:D3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1528,9 +1528,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1698,19 +1701,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1EC9FDFB-29C9-4D71-A78D-DC63A8164647}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1CA316B-A5FF-4AE2-9421-20955EA2F4E1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1734,9 +1733,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1CA316B-A5FF-4AE2-9421-20955EA2F4E1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1EC9FDFB-29C9-4D71-A78D-DC63A8164647}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>